<commit_message>
add measurement on rubber, etc
</commit_message>
<xml_diff>
--- a/Measurements/018 damper and joint/measurements.xlsx
+++ b/Measurements/018 damper and joint/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e5a9c027fd1ff47/Desktop/Meng/solidworks/Measurements/018 damper and joint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="492" documentId="13_ncr:1_{C0D69B80-9267-4075-BE2F-A7C77B285423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B0615D-D09D-4BA8-AB87-76DFE8CE2057}"/>
+  <xr:revisionPtr revIDLastSave="570" documentId="13_ncr:1_{C0D69B80-9267-4075-BE2F-A7C77B285423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FF50323-2FD7-4441-A234-5C42408BA356}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="192">
   <si>
     <t>Measuring Instrument Verification Record</t>
   </si>
@@ -574,6 +574,45 @@
   </si>
   <si>
     <t>2.5060</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Loc 1</t>
+  </si>
+  <si>
+    <t>Loc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loc 3 </t>
+  </si>
+  <si>
+    <t>Loc 4</t>
+  </si>
+  <si>
+    <t>Loc 5</t>
+  </si>
+  <si>
+    <t>Loc 6</t>
+  </si>
+  <si>
+    <t>Loc 7</t>
+  </si>
+  <si>
+    <t>Loc 8</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>61</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1040,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1131,13 +1170,49 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3715,11 +3790,547 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>383617</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B9D198-8AEC-4376-BF40-BF1836A57D10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10467975" y="2705100"/>
+          <a:ext cx="3136342" cy="2771775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>339224</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57652</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A3D81A-AD4E-41BE-92B3-EAFD6AAADC02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11159624" y="3562852"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>62999</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19552</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FF14ABF-7E66-426B-A6EE-85D40E8D80D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12083549" y="3277102"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>62999</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19552</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9529C639-63A4-4D99-99B4-88A6724856B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11483474" y="3277102"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>472574</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76702</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextBox 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9905EFB8-80CF-4FAA-910D-040B06B31F40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12493124" y="3581902"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>491624</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133852</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABC68D7-071C-4974-AF1B-EC51FC71DF93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12512174" y="4382002"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>5</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>205874</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152902</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABFB3A5D-766A-4049-B32E-C0F9F269D537}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12226424" y="4648702"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>6</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>348749</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>67177</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="TextBox 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6ED631E-8467-4E4A-9233-CF7EFEEF9788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11169149" y="4315327"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>8</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>91574</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>143377</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="TextBox 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A90813-58EB-4D8A-85C7-2A58FA875E37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11512049" y="4639177"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>7</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3995,21 +4606,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:13" ht="26.45" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -4663,7 +5274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C688C08-1670-4A69-A539-D119A5695C86}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
@@ -4676,21 +5287,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:13" ht="26.45" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -5335,7 +5946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3ECA65-3337-4C9B-9652-F5F135591ACE}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -5345,10 +5956,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -5954,7 +6565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0680577E-1C62-49B4-BCA6-3E2C997F9A41}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
@@ -5964,10 +6575,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -6763,10 +7374,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0831657-1486-4553-AB4D-7EEB3D0DF771}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
@@ -6777,24 +7388,24 @@
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:23" ht="30" customHeight="1">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-    </row>
-    <row r="2" spans="1:13" ht="26.45" customHeight="1" thickBot="1">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+    </row>
+    <row r="2" spans="1:23" ht="26.45" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -6813,7 +7424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="24.95" customHeight="1" thickTop="1">
+    <row r="3" spans="1:23" ht="24.95" customHeight="1" thickTop="1">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -6845,8 +7456,35 @@
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
       <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="O3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -6878,8 +7516,35 @@
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
       <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+      <c r="P4" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q4" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="R4" s="47">
+        <v>64</v>
+      </c>
+      <c r="S4" s="48">
+        <v>65</v>
+      </c>
+      <c r="T4" s="48">
+        <v>65</v>
+      </c>
+      <c r="U4" s="48">
+        <v>54</v>
+      </c>
+      <c r="V4" s="48">
+        <v>65</v>
+      </c>
+      <c r="W4" s="49">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -6904,15 +7569,42 @@
       <c r="H5" s="23">
         <v>1.224</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="43">
         <v>67</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="27"/>
-    </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="O5" s="7">
+        <v>2</v>
+      </c>
+      <c r="P5" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q5" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="R5" s="47">
+        <v>61</v>
+      </c>
+      <c r="S5" s="51">
+        <v>62</v>
+      </c>
+      <c r="T5" s="51">
+        <v>62</v>
+      </c>
+      <c r="U5" s="51">
+        <v>61</v>
+      </c>
+      <c r="V5" s="51">
+        <v>62</v>
+      </c>
+      <c r="W5" s="52">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -6937,15 +7629,42 @@
       <c r="H6" s="23">
         <v>1.2195</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="43">
         <v>67</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="27"/>
-    </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="O6" s="7">
+        <v>3</v>
+      </c>
+      <c r="P6" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q6" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="R6" s="53">
+        <v>64</v>
+      </c>
+      <c r="S6" s="51">
+        <v>64</v>
+      </c>
+      <c r="T6" s="51">
+        <v>64</v>
+      </c>
+      <c r="U6" s="51">
+        <v>62</v>
+      </c>
+      <c r="V6" s="51">
+        <v>64</v>
+      </c>
+      <c r="W6" s="52">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -6970,15 +7689,42 @@
       <c r="H7" s="23">
         <v>1.2190000000000001</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="43">
         <v>67</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="27"/>
-    </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="O7" s="7">
+        <v>4</v>
+      </c>
+      <c r="P7" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q7" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="R7" s="53">
+        <v>64</v>
+      </c>
+      <c r="S7" s="51">
+        <v>64</v>
+      </c>
+      <c r="T7" s="51">
+        <v>63</v>
+      </c>
+      <c r="U7" s="51">
+        <v>64</v>
+      </c>
+      <c r="V7" s="51">
+        <v>63</v>
+      </c>
+      <c r="W7" s="52">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="26">
         <v>5</v>
       </c>
@@ -7003,16 +7749,47 @@
       <c r="H8" s="24">
         <v>1.2224999999999999</v>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="44">
         <v>67</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="25"/>
-    </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1"/>
-    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="O8" s="26">
+        <v>5</v>
+      </c>
+      <c r="P8" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q8" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="R8" s="55">
+        <v>64</v>
+      </c>
+      <c r="S8" s="56">
+        <v>64</v>
+      </c>
+      <c r="T8" s="56">
+        <v>64</v>
+      </c>
+      <c r="U8" s="56">
+        <v>64</v>
+      </c>
+      <c r="V8" s="56">
+        <v>64</v>
+      </c>
+      <c r="W8" s="57">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="20.100000000000001" customHeight="1" thickTop="1">
+      <c r="O9" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -7027,7 +7804,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -7042,7 +7819,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -7057,7 +7834,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -7074,7 +7851,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -7089,7 +7866,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -7104,7 +7881,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:23" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>

</xml_diff>